<commit_message>
Programme Done - Without JDOC
</commit_message>
<xml_diff>
--- a/out/production/ArlaKPI/Resources/Files/Data2.xlsx
+++ b/out/production/ArlaKPI/Resources/Files/Data2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Produktions Quota</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>Mælk</t>
+    <t>Mælkebøtte</t>
   </si>
   <si>
     <t>Cocio</t>
@@ -48,12 +48,15 @@
   <si>
     <t>Is</t>
   </si>
+  <si>
+    <t>Flute</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -64,6 +67,10 @@
       <color theme="1"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -79,12 +86,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -330,7 +343,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1">
@@ -415,37 +428,54 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>250.0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>300.0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>550.0</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>150.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>250.0</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>350.0</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>450.0</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>100.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>800.0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>200.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>10.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>